<commit_message>
Fixed most of the logic errors. Added a graph to show the final data. The credits for each semester are still at 18 and need to be smaller if possible.
</commit_message>
<xml_diff>
--- a/data/Classes.xlsx
+++ b/data/Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielanderson/Documents/class_scheduler/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678F4C54-97A6-8848-A017-5C2667B47358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D68EA4B-BC71-2744-9D5A-1C013E0426BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="283">
   <si>
     <t>Course</t>
   </si>
@@ -818,9 +818,6 @@
     <t>Spring A, Summer A</t>
   </si>
   <si>
-    <t>BUSN 319; BUSN 320; BUSN 323; BUSN 347; BUSN  361; BUSN 370; BUSN 376; BUSN 422</t>
-  </si>
-  <si>
     <t>course</t>
   </si>
   <si>
@@ -837,6 +834,51 @@
   </si>
   <si>
     <t>credits</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Fall A, Fall B, Spring A, Spring B</t>
+  </si>
+  <si>
+    <t>Fall A, Fall B, Spring A, Spring B, Summer B</t>
+  </si>
+  <si>
+    <t>Fall B, Spring A, Summer A</t>
+  </si>
+  <si>
+    <t>Spring B, Summer A</t>
+  </si>
+  <si>
+    <t>Fall A, Spring A</t>
+  </si>
+  <si>
+    <t>Summer A, Summer B</t>
+  </si>
+  <si>
+    <t>Fall A, Spring A, Summer A</t>
+  </si>
+  <si>
+    <t>Fall B, Spring B, Summer B</t>
+  </si>
+  <si>
+    <t>Fall B, Spring B, Summer A, Summer B</t>
+  </si>
+  <si>
+    <t>Fall Full</t>
+  </si>
+  <si>
+    <t>Fall Full, Spring Full, Summer Full</t>
+  </si>
+  <si>
+    <t>Fall A, Summer A</t>
+  </si>
+  <si>
+    <t>Fall A, Spring A, Summer B</t>
+  </si>
+  <si>
+    <t>BUSN 319; BUSN 320; BUSN 323; BUSN 347; BUSN 361; BUSN 370; BUSN 376; BUSN 422</t>
   </si>
 </sst>
 </file>
@@ -1657,6 +1699,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1674,9 +1719,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1895,11 +1937,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1916,13 +1958,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="233" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="233" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="233" t="s">
+      <c r="C1" s="233" t="s">
         <v>264</v>
-      </c>
-      <c r="C1" s="233" t="s">
-        <v>265</v>
       </c>
       <c r="D1" s="233" t="s">
         <v>254</v>
@@ -1931,13 +1973,13 @@
         <v>255</v>
       </c>
       <c r="F1" s="233" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" s="234" t="s">
+        <v>267</v>
+      </c>
+      <c r="H1" s="233" t="s">
         <v>266</v>
-      </c>
-      <c r="G1" s="241" t="s">
-        <v>268</v>
-      </c>
-      <c r="H1" s="233" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
@@ -2242,8 +2284,8 @@
       <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>262</v>
+      <c r="C16" s="232" t="s">
+        <v>282</v>
       </c>
       <c r="D16" t="s">
         <v>243</v>
@@ -2255,6 +2297,439 @@
         <v>1</v>
       </c>
       <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="232" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="232" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="232" t="s">
+        <v>269</v>
+      </c>
+      <c r="E17" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="232">
+        <v>1</v>
+      </c>
+      <c r="G17" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="232" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="232" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="232" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18" s="232">
+        <v>1</v>
+      </c>
+      <c r="G18" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="232" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="232" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="232" t="s">
+        <v>271</v>
+      </c>
+      <c r="E19" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F19" s="232">
+        <v>1</v>
+      </c>
+      <c r="G19" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="232" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="232" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="232" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F20" s="232">
+        <v>1</v>
+      </c>
+      <c r="G20" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="232" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="232" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="232" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="232" t="s">
+        <v>272</v>
+      </c>
+      <c r="E21" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F21" s="232">
+        <v>1</v>
+      </c>
+      <c r="G21" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" s="232" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="232" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="232" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="232" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="232">
+        <v>1</v>
+      </c>
+      <c r="G22" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A23" s="232" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="232" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="232" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" s="232">
+        <v>1</v>
+      </c>
+      <c r="G23" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A24" s="232" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="232" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="232" t="s">
+        <v>275</v>
+      </c>
+      <c r="E24" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F24" s="232">
+        <v>1</v>
+      </c>
+      <c r="G24" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A25" s="232" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="232" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="232" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F25" s="232">
+        <v>1</v>
+      </c>
+      <c r="G25" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A26" s="232" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="232" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="232" t="s">
+        <v>277</v>
+      </c>
+      <c r="E26" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F26" s="232">
+        <v>1</v>
+      </c>
+      <c r="G26" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A27" s="232" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="232" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="232" t="s">
+        <v>278</v>
+      </c>
+      <c r="E27" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F27" s="232">
+        <v>1</v>
+      </c>
+      <c r="G27" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A28" s="232" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="232" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="232" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F28" s="232">
+        <v>1</v>
+      </c>
+      <c r="G28" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A29" s="232" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="232" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="232" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="232" t="s">
+        <v>279</v>
+      </c>
+      <c r="E29" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F29" s="232">
+        <v>1</v>
+      </c>
+      <c r="G29" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A30" s="232" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="232" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="232" t="s">
+        <v>275</v>
+      </c>
+      <c r="E30" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F30" s="232">
+        <v>1</v>
+      </c>
+      <c r="G30" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A31" s="232" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="232" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="232" t="s">
+        <v>278</v>
+      </c>
+      <c r="E31" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31" s="232">
+        <v>1</v>
+      </c>
+      <c r="G31" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A32" s="232" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="232" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="232" t="s">
+        <v>242</v>
+      </c>
+      <c r="E32" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F32" s="232">
+        <v>1</v>
+      </c>
+      <c r="G32" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A33" s="232" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="232" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="232"/>
+      <c r="D33" s="232" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F33" s="232">
+        <v>1</v>
+      </c>
+      <c r="G33" s="232">
+        <v>3</v>
+      </c>
+      <c r="H33" s="232" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A34" s="232" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="232" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="232" t="s">
+        <v>280</v>
+      </c>
+      <c r="E34" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" s="232">
+        <v>1</v>
+      </c>
+      <c r="G34" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A35" s="232" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="232" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="232" t="s">
+        <v>281</v>
+      </c>
+      <c r="E35" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F35" s="232">
+        <v>1</v>
+      </c>
+      <c r="G35" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A36" s="232" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="232" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="232" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F36" s="232">
+        <v>1</v>
+      </c>
+      <c r="G36" s="232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A37" s="232" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="232" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="232" t="s">
+        <v>243</v>
+      </c>
+      <c r="E37" s="232" t="s">
+        <v>256</v>
+      </c>
+      <c r="F37" s="232">
+        <v>1</v>
+      </c>
+      <c r="G37" s="232">
         <v>3</v>
       </c>
     </row>
@@ -2273,6 +2748,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="232" t="s">
@@ -2449,21 +2927,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="11" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.5" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2722,6 +3205,186 @@
       <c r="L7" s="4" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A12" s="233" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="233" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="233" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="233" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="233" t="s">
+        <v>255</v>
+      </c>
+      <c r="F12" s="233" t="s">
+        <v>265</v>
+      </c>
+      <c r="G12" s="234" t="s">
+        <v>267</v>
+      </c>
+      <c r="H12" s="233" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" t="s">
+        <v>256</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2734,7 +3397,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3326,6 +3989,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -31676,14 +32340,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.5" customHeight="1">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="235"/>
-      <c r="C1" s="235"/>
-      <c r="D1" s="235"/>
-      <c r="E1" s="235"/>
-      <c r="F1" s="235"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
     </row>
     <row r="2" spans="1:13" ht="13">
       <c r="A2" s="184" t="s">
@@ -31913,18 +32577,18 @@
       <c r="G14" s="190"/>
     </row>
     <row r="15" spans="1:13" ht="13">
-      <c r="A15" s="236" t="s">
+      <c r="A15" s="237" t="s">
         <v>233</v>
       </c>
-      <c r="B15" s="235"/>
-      <c r="C15" s="237" t="s">
+      <c r="B15" s="236"/>
+      <c r="C15" s="238" t="s">
         <v>234</v>
       </c>
-      <c r="D15" s="235"/>
-      <c r="E15" s="238" t="s">
+      <c r="D15" s="236"/>
+      <c r="E15" s="239" t="s">
         <v>235</v>
       </c>
-      <c r="F15" s="235"/>
+      <c r="F15" s="236"/>
       <c r="G15" s="190"/>
     </row>
     <row r="16" spans="1:13" ht="13">
@@ -31932,14 +32596,14 @@
         <v>236</v>
       </c>
       <c r="B16" s="213"/>
-      <c r="C16" s="239" t="s">
+      <c r="C16" s="240" t="s">
         <v>237</v>
       </c>
-      <c r="D16" s="235"/>
-      <c r="E16" s="240" t="s">
+      <c r="D16" s="236"/>
+      <c r="E16" s="241" t="s">
         <v>238</v>
       </c>
-      <c r="F16" s="235"/>
+      <c r="F16" s="236"/>
       <c r="G16" s="190"/>
       <c r="H16" s="214"/>
       <c r="I16" s="215"/>

</xml_diff>